<commit_message>
chore: Update tests after updating general sheet with thermo/flux priors
</commit_message>
<xml_diff>
--- a/matlab_code/tests/analysisFxns/testFiles/toy_model1_numbers.xlsx
+++ b/matlab_code/tests/analysisFxns/testFiles/toy_model1_numbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="104">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t xml:space="preserve">gurobi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior distribution for fluxes (uniform or normal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior distribution for thermodynamic quantities (uniform or normal)</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
@@ -424,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,6 +444,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -472,8 +485,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,64 +535,78 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -600,7 +627,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A6:B7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,21 +637,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938745891927311</v>
@@ -638,7 +665,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.918129270809538</v>
@@ -652,7 +679,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.979330692978098</v>
@@ -666,7 +693,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.870960152966783</v>
@@ -680,7 +707,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.99</v>
@@ -694,7 +721,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -708,7 +735,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -722,7 +749,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -736,7 +763,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -750,7 +777,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -764,7 +791,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -778,7 +805,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -792,7 +819,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -823,7 +850,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A6:B7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -833,21 +860,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.729362608113343</v>
@@ -861,7 +888,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -875,7 +902,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -889,7 +916,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -903,7 +930,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -917,7 +944,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.985171462369796</v>
@@ -931,7 +958,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.875198318353468</v>
@@ -945,7 +972,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.992232956019871</v>
@@ -959,7 +986,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.87219768970854</v>
@@ -973,7 +1000,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.997064475108798</v>
@@ -987,7 +1014,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1001,7 +1028,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.935839477601494</v>
@@ -1015,7 +1042,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1029,7 +1056,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1043,7 +1070,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.864112211147392</v>
@@ -1057,7 +1084,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1071,7 +1098,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1085,7 +1112,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.980827889050257</v>
@@ -1099,7 +1126,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.983205843276524</v>
@@ -1113,7 +1140,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.986809036820528</v>
@@ -1143,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="1" sqref="A6:B7 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1160,57 +1187,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1221,19 +1248,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1244,22 +1271,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1270,16 +1297,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1290,19 +1317,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1313,22 +1340,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1339,10 +1366,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1353,10 +1380,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1367,10 +1394,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1381,10 +1408,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1395,10 +1422,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1409,10 +1436,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1423,10 +1450,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1454,7 +1481,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="A6:B7 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1464,72 +1491,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1594,7 +1621,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1659,7 +1686,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1724,7 +1751,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1789,7 +1816,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1854,7 +1881,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-1</v>
@@ -1919,7 +1946,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -1984,7 +2011,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2049,7 +2076,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2114,7 +2141,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2179,7 +2206,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2244,7 +2271,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2309,7 +2336,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2391,7 +2418,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A6:B7 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2402,21 +2429,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2424,10 +2451,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2435,10 +2462,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2446,10 +2473,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2457,10 +2484,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2468,10 +2495,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2479,10 +2506,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2490,10 +2517,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2501,10 +2528,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2512,10 +2539,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2523,10 +2550,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2534,10 +2561,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2545,10 +2572,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2556,10 +2583,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2567,10 +2594,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2578,10 +2605,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2589,10 +2616,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -2600,10 +2627,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -2611,10 +2638,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -2622,10 +2649,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -2650,7 +2677,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A6:B7 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2661,24 +2688,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2686,10 +2713,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2697,10 +2724,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2708,10 +2735,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2719,10 +2746,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -2730,10 +2757,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -2741,10 +2768,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -2752,10 +2779,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -2763,10 +2790,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -2774,10 +2801,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -2785,10 +2812,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -2796,10 +2823,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2807,10 +2834,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2835,7 +2862,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A6:B7 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2845,107 +2872,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2967,7 +2994,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A6:B7 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2977,107 +3004,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3099,7 +3126,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A6:B7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3109,18 +3136,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3131,7 +3158,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3142,7 +3169,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3153,7 +3180,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3164,7 +3191,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-43.2</v>
@@ -3175,7 +3202,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-24.6</v>
@@ -3186,7 +3213,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-40</v>
@@ -3197,7 +3224,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-10</v>
@@ -3208,7 +3235,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-30</v>
@@ -3219,7 +3246,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-10</v>
@@ -3230,7 +3257,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3241,7 +3268,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3252,7 +3279,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3280,7 +3307,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A6:B7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3290,18 +3317,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.65155467201437E-005</v>
@@ -3312,7 +3339,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3323,7 +3350,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3334,7 +3361,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3345,7 +3372,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3356,7 +3383,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00161010544336061</v>
@@ -3367,7 +3394,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.0018583615823201</v>
@@ -3378,7 +3405,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00102168275785283</v>
@@ -3389,7 +3416,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0171065051554435</v>
@@ -3400,7 +3427,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00285146987847134</v>
@@ -3411,7 +3438,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1E-012</v>
@@ -3422,7 +3449,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0013710175574537</v>
@@ -3433,7 +3460,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -3444,7 +3471,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -3455,7 +3482,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.37459615540709E-005</v>
@@ -3466,7 +3493,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -3477,7 +3504,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1E-012</v>
@@ -3488,7 +3515,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6.69219105835325E-006</v>
@@ -3499,7 +3526,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.00351539405111918</v>
@@ -3510,7 +3537,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.000588959799304437</v>
@@ -3538,7 +3565,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A6:B7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3551,18 +3578,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-22.0149320730417</v>
@@ -3574,7 +3601,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.285369137837419</v>
@@ -3586,7 +3613,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0578197638950879</v>
@@ -3598,7 +3625,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.00439408376660814</v>
@@ -3610,7 +3637,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.84865633256387</v>
@@ -3622,7 +3649,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.00242684925806694</v>

</xml_diff>